<commit_message>
macro to save each sheet in csv
</commit_message>
<xml_diff>
--- a/Vivekananda.xlsx
+++ b/Vivekananda.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\swami-vivekananda-quotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26976E94-611B-4088-8237-B6F9566202DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BE09E4-9917-4FC2-8C7E-518EA8B58866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="1" r:id="rId1"/>
@@ -1558,10 +1558,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="45.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1926,9 +1927,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363F57CC-7BFF-42B5-8659-A4D423D2D3F6}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2300,9 +2302,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760FD0F7-5BE9-4FF1-BFB6-671E531BF41D}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -2692,9 +2695,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F47B088-CC2D-415B-9AE9-E9943FC1851A}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C20" activeCellId="1" sqref="C21 C20"/>
     </sheetView>
   </sheetViews>
@@ -3093,9 +3097,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EC8C9C-1882-4AC5-8D7F-12EB4CACDF72}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -3259,6 +3264,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E330C11-EC7D-4988-8B54-7A59B49482E1}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -3646,6 +3652,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B06F4B-35A6-4B4B-BDEF-BA1206D9DA9B}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3867,10 +3874,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B0EF2B-B739-41CE-A86F-6F28CC3FF522}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C30"/>
+    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3894,6 +3902,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>108</v>
       </c>
@@ -3903,6 +3914,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>109</v>
       </c>
@@ -3912,6 +3926,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>110</v>
       </c>
@@ -3921,6 +3938,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>111</v>
       </c>
@@ -3930,6 +3950,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>112</v>
       </c>
@@ -3939,6 +3962,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>113</v>
       </c>
@@ -3948,6 +3974,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>114</v>
       </c>
@@ -3957,6 +3986,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>115</v>
       </c>
@@ -3966,6 +3998,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>116</v>
       </c>
@@ -3975,6 +4010,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>117</v>
       </c>
@@ -3984,6 +4022,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>118</v>
       </c>
@@ -3993,6 +4034,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>119</v>
       </c>
@@ -4005,6 +4049,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>121</v>
       </c>
@@ -4014,6 +4061,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>122</v>
       </c>
@@ -4023,6 +4073,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>123</v>
       </c>
@@ -4031,7 +4084,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>124</v>
       </c>
@@ -4040,7 +4096,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>125</v>
       </c>
@@ -4049,7 +4108,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>126</v>
       </c>
@@ -4058,7 +4120,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
       <c r="B20" s="3" t="s">
         <v>127</v>
       </c>
@@ -4067,7 +4132,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
       <c r="B21" s="3" t="s">
         <v>128</v>
       </c>
@@ -4076,7 +4144,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>129</v>
       </c>
@@ -4085,7 +4156,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
       <c r="B23" s="3" t="s">
         <v>130</v>
       </c>
@@ -4094,7 +4168,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>131</v>
       </c>
@@ -4103,7 +4180,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
       <c r="B25" s="3" t="s">
         <v>132</v>
       </c>
@@ -4112,7 +4192,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>133</v>
       </c>
@@ -4121,7 +4204,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>134</v>
       </c>
@@ -4130,7 +4216,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
       <c r="B28" s="3" t="s">
         <v>135</v>
       </c>
@@ -4139,7 +4228,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
       <c r="B29" s="3" t="s">
         <v>136</v>
       </c>
@@ -4148,7 +4240,10 @@
         <v>April</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
       <c r="B30" s="3" t="s">
         <v>137</v>
       </c>
@@ -4164,10 +4259,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724FB1A4-20EA-4293-985A-C5F55F03FE25}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4191,6 +4287,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>138</v>
       </c>
@@ -4200,6 +4299,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>139</v>
       </c>
@@ -4209,6 +4311,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>140</v>
       </c>
@@ -4218,6 +4323,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>141</v>
       </c>
@@ -4227,6 +4335,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>142</v>
       </c>
@@ -4236,6 +4347,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>143</v>
       </c>
@@ -4245,6 +4359,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>144</v>
       </c>
@@ -4254,6 +4371,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>145</v>
       </c>
@@ -4263,6 +4383,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>146</v>
       </c>
@@ -4272,6 +4395,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>147</v>
       </c>
@@ -4281,6 +4407,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>148</v>
       </c>
@@ -4290,6 +4419,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>149</v>
       </c>
@@ -4299,6 +4431,9 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>150</v>
       </c>
@@ -4308,6 +4443,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>151</v>
       </c>
@@ -4317,6 +4455,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>152</v>
       </c>
@@ -4325,7 +4466,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>153</v>
       </c>
@@ -4334,7 +4478,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>154</v>
       </c>
@@ -4343,7 +4490,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>155</v>
       </c>
@@ -4355,7 +4505,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
       <c r="B20" s="3" t="s">
         <v>157</v>
       </c>
@@ -4364,7 +4517,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
       <c r="B21" s="3" t="s">
         <v>158</v>
       </c>
@@ -4373,7 +4529,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>159</v>
       </c>
@@ -4382,7 +4541,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
       <c r="B23" s="3" t="s">
         <v>160</v>
       </c>
@@ -4391,7 +4553,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>161</v>
       </c>
@@ -4400,7 +4565,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
       <c r="B25" s="3" t="s">
         <v>162</v>
       </c>
@@ -4409,7 +4577,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>163</v>
       </c>
@@ -4418,7 +4589,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>164</v>
       </c>
@@ -4427,7 +4601,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
       <c r="B28" s="3" t="s">
         <v>165</v>
       </c>
@@ -4436,7 +4613,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
       <c r="B29" s="3" t="s">
         <v>166</v>
       </c>
@@ -4445,7 +4625,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
       <c r="B30" s="3" t="s">
         <v>167</v>
       </c>
@@ -4454,7 +4637,10 @@
         <v>May</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
       <c r="B31" s="3" t="s">
         <v>168</v>
       </c>
@@ -4471,10 +4657,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11142260-1394-466E-A210-029EEC0502F2}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4498,6 +4685,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>169</v>
       </c>
@@ -4507,6 +4697,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>170</v>
       </c>
@@ -4516,6 +4709,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>171</v>
       </c>
@@ -4525,6 +4721,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>172</v>
       </c>
@@ -4534,6 +4733,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>173</v>
       </c>
@@ -4543,6 +4745,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>174</v>
       </c>
@@ -4552,6 +4757,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>175</v>
       </c>
@@ -4561,6 +4769,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>176</v>
       </c>
@@ -4570,6 +4781,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>177</v>
       </c>
@@ -4582,6 +4796,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>179</v>
       </c>
@@ -4591,6 +4808,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>180</v>
       </c>
@@ -4600,6 +4820,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>181</v>
       </c>
@@ -4609,6 +4832,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>182</v>
       </c>
@@ -4618,6 +4844,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>183</v>
       </c>
@@ -4627,6 +4856,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>184</v>
       </c>
@@ -4635,7 +4867,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>185</v>
       </c>
@@ -4644,7 +4879,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>186</v>
       </c>
@@ -4653,7 +4891,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>187</v>
       </c>
@@ -4662,7 +4903,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
       <c r="B20" s="3" t="s">
         <v>188</v>
       </c>
@@ -4671,7 +4915,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
       <c r="B21" s="3" t="s">
         <v>189</v>
       </c>
@@ -4680,7 +4927,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>190</v>
       </c>
@@ -4689,7 +4939,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
       <c r="B23" s="3" t="s">
         <v>191</v>
       </c>
@@ -4698,7 +4951,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>192</v>
       </c>
@@ -4707,7 +4963,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
       <c r="B25" s="3" t="s">
         <v>193</v>
       </c>
@@ -4716,7 +4975,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>194</v>
       </c>
@@ -4725,7 +4987,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>195</v>
       </c>
@@ -4734,7 +4999,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
       <c r="B28" s="3" t="s">
         <v>196</v>
       </c>
@@ -4746,7 +5014,10 @@
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
       <c r="B29" s="3" t="s">
         <v>198</v>
       </c>
@@ -4755,7 +5026,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
       <c r="B30" s="3" t="s">
         <v>199</v>
       </c>
@@ -4764,7 +5038,10 @@
         <v>June</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
       <c r="B31" s="3" t="s">
         <v>200</v>
       </c>
@@ -4780,10 +5057,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0F0144-0E7B-4C5A-A6C9-3327949F7E86}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4806,6 +5084,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>210</v>
       </c>
@@ -4815,6 +5096,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>211</v>
       </c>
@@ -4824,6 +5108,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>212</v>
       </c>
@@ -4833,6 +5120,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>213</v>
       </c>
@@ -4842,6 +5132,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>214</v>
       </c>
@@ -4851,6 +5144,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>215</v>
       </c>
@@ -4860,6 +5156,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>216</v>
       </c>
@@ -4869,6 +5168,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>217</v>
       </c>
@@ -4878,6 +5180,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>218</v>
       </c>
@@ -4887,6 +5192,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>219</v>
       </c>
@@ -4896,6 +5204,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>220</v>
       </c>
@@ -4905,6 +5216,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>221</v>
       </c>
@@ -4914,6 +5228,9 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>222</v>
       </c>
@@ -4923,6 +5240,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>223</v>
       </c>
@@ -4932,6 +5252,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>224</v>
       </c>
@@ -4940,7 +5263,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>225</v>
       </c>
@@ -4949,7 +5275,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>226</v>
       </c>
@@ -4958,7 +5287,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>227</v>
       </c>
@@ -4967,7 +5299,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
       <c r="B20" s="3" t="s">
         <v>228</v>
       </c>
@@ -4976,7 +5311,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
       <c r="B21" s="3" t="s">
         <v>229</v>
       </c>
@@ -4985,7 +5323,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>230</v>
       </c>
@@ -4994,7 +5335,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
       <c r="B23" s="3" t="s">
         <v>231</v>
       </c>
@@ -5003,7 +5347,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>232</v>
       </c>
@@ -5012,7 +5359,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
       <c r="B25" s="3" t="s">
         <v>233</v>
       </c>
@@ -5021,7 +5371,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>234</v>
       </c>
@@ -5030,7 +5383,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>235</v>
       </c>
@@ -5039,7 +5395,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
       <c r="B28" s="3" t="s">
         <v>236</v>
       </c>
@@ -5048,7 +5407,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
       <c r="B29" s="3" t="s">
         <v>237</v>
       </c>
@@ -5057,7 +5419,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
       <c r="B30" s="3" t="s">
         <v>238</v>
       </c>
@@ -5066,7 +5431,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
       <c r="B31" s="3" t="s">
         <v>239</v>
       </c>
@@ -5075,7 +5443,10 @@
         <v>July</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
       <c r="B32" s="3" t="s">
         <v>240</v>
       </c>
@@ -5091,10 +5462,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE62583-A7A2-4F1A-B8AB-7CEEE007B4E0}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5117,6 +5489,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>241</v>
       </c>
@@ -5126,6 +5501,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>242</v>
       </c>
@@ -5135,6 +5513,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>243</v>
       </c>
@@ -5144,6 +5525,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>244</v>
       </c>
@@ -5153,6 +5537,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>245</v>
       </c>
@@ -5162,6 +5549,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>246</v>
       </c>
@@ -5171,6 +5561,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>247</v>
       </c>
@@ -5180,6 +5573,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>248</v>
       </c>
@@ -5189,6 +5585,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>249</v>
       </c>
@@ -5198,6 +5597,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>250</v>
       </c>
@@ -5207,6 +5609,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>251</v>
       </c>
@@ -5216,6 +5621,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>252</v>
       </c>
@@ -5225,6 +5633,9 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>253</v>
       </c>
@@ -5234,6 +5645,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>254</v>
       </c>
@@ -5243,6 +5657,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>255</v>
       </c>
@@ -5251,7 +5668,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>256</v>
       </c>
@@ -5260,7 +5680,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>257</v>
       </c>
@@ -5269,7 +5692,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>258</v>
       </c>
@@ -5278,7 +5704,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
       <c r="B20" s="3" t="s">
         <v>259</v>
       </c>
@@ -5287,7 +5716,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
       <c r="B21" s="3" t="s">
         <v>260</v>
       </c>
@@ -5296,7 +5728,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>261</v>
       </c>
@@ -5305,7 +5740,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
       <c r="B23" s="3" t="s">
         <v>262</v>
       </c>
@@ -5314,7 +5752,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>263</v>
       </c>
@@ -5323,7 +5764,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
       <c r="B25" s="3" t="s">
         <v>264</v>
       </c>
@@ -5332,7 +5776,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>265</v>
       </c>
@@ -5341,7 +5788,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>266</v>
       </c>
@@ -5350,7 +5800,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
       <c r="B28" s="3" t="s">
         <v>267</v>
       </c>
@@ -5359,7 +5812,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
       <c r="B29" s="3" t="s">
         <v>268</v>
       </c>
@@ -5368,7 +5824,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
       <c r="B30" s="3" t="s">
         <v>269</v>
       </c>
@@ -5377,7 +5836,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
       <c r="B31" s="3" t="s">
         <v>270</v>
       </c>
@@ -5386,7 +5848,10 @@
         <v>August</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
       <c r="B32" s="3" t="s">
         <v>201</v>
       </c>
@@ -5403,9 +5868,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07B24EC-ECE8-4C19-A2BA-51143D3C8B21}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>